<commit_message>
Andy: add item to script #1 and update data sources (xlsx)
</commit_message>
<xml_diff>
--- a/Resources/1-Datastore.xlsx
+++ b/Resources/1-Datastore.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
   <si>
     <t>Customer</t>
   </si>
@@ -172,13 +172,40 @@
   </si>
   <si>
     <t>Acushnet#1</t>
+  </si>
+  <si>
+    <t>06Y Flagship</t>
+  </si>
+  <si>
+    <t>US00060736</t>
+  </si>
+  <si>
+    <t>Color Sku</t>
+  </si>
+  <si>
+    <t>TB7SX14CC-016</t>
+  </si>
+  <si>
+    <t>ConfigB5</t>
+  </si>
+  <si>
+    <t>ss</t>
+  </si>
+  <si>
+    <t>TB7SX14CC</t>
+  </si>
+  <si>
+    <t>TB7SX7SC</t>
+  </si>
+  <si>
+    <t>US00064622</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,13 +227,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -221,11 +268,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -765,10 +815,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,13 +827,14 @@
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -811,8 +862,14 @@
       <c r="I1" t="s">
         <v>49</v>
       </c>
+      <c r="J1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -841,14 +898,34 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F3" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F4" s="2" t="s">
-        <v>47</v>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="K4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>